<commit_message>
First attempt to run as shiny app
Yair commits it
</commit_message>
<xml_diff>
--- a/Data/fields.xlsx
+++ b/Data/fields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hujiacil-my.sharepoint.com/personal/noamgrid_on_huji_ac_il/Documents/PhD/projects/TaxoTox/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yair\Documents\yair\research\estuary_rehabilitation\yairs_stuff\Students\Noam\TaxoTox\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_B89231273C9967F8C8B5B8DDAB3E0806FA5B91EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22DBAA4-D98C-4C8A-AF67-977A13F51980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2414,10 +2414,13 @@
   <dimension ref="A1:A686"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
-      <selection activeCell="G593" sqref="G593"/>
+      <selection activeCell="A580" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>